<commit_message>
CSV files with lda only, bayes only and both comparison
</commit_message>
<xml_diff>
--- a/results/results_lot_00_graphs.xlsx
+++ b/results/results_lot_00_graphs.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/57546c4bddaabca5/Documents/School/SchoolYears/Senior Year/CSC200H/Projects/FakeNews/results/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\OneDrive\Documents\School\SchoolYears\Senior Year\CSC200H\Projects\FakeNews\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="accuracy all" sheetId="2" r:id="rId1"/>
     <sheet name="accuracy avg" sheetId="3" r:id="rId2"/>
     <sheet name="results_lot_00" sheetId="1" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -7825,6 +7825,7 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="r"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -7842,20 +7843,6 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -7912,7 +7899,7 @@
           </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
+        <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
@@ -8029,7 +8016,7 @@
           </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
+        <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
@@ -8078,7 +8065,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="b"/>
+      <c:legendPos val="r"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9267,7 +9254,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="71" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="86" workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -9639,8 +9626,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I351"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>